<commit_message>
atualização dos documentos do SIB 5
</commit_message>
<xml_diff>
--- a/Requisitos/Definição de prioridade.xlsx
+++ b/Requisitos/Definição de prioridade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josimar\Documents\GitHub\SIB\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -190,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -198,20 +198,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -521,7 +563,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +578,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -559,176 +601,176 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>B2*C2</f>
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <f>D2*E2*F2</f>
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D8" si="0">B3*C3</f>
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G8" si="1">D3*E3*F3</f>
         <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>B4*C4</f>
         <v>9</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>

</xml_diff>